<commit_message>
added mac verification, added yaml template file for port mapping columns
</commit_message>
<xml_diff>
--- a/host_list.xlsx
+++ b/host_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doug.colthar\PycharmProjects\napalm_tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doug.colthar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84597A2-8F04-4A28-A12E-ED1F02916413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4A187D-C884-404E-B84D-752C91B2CE09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F6230A2-FC52-421C-BE82-43F4E2C1777E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F6230A2-FC52-421C-BE82-43F4E2C1777E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>IP Address</t>
   </si>
@@ -59,28 +59,49 @@
     <t>Closet Name</t>
   </si>
   <si>
-    <t>MDF</t>
-  </si>
-  <si>
-    <t>IDF1</t>
-  </si>
-  <si>
-    <t>HQ</t>
-  </si>
-  <si>
-    <t>test_core1</t>
-  </si>
-  <si>
-    <t>Branch1</t>
-  </si>
-  <si>
-    <t>172.16.50.10</t>
-  </si>
-  <si>
     <t>172.16.1.1</t>
   </si>
   <si>
-    <t>test_access1</t>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>RH.1.S1</t>
+  </si>
+  <si>
+    <t>RH.1.Petit</t>
+  </si>
+  <si>
+    <t>RH.1.E1</t>
+  </si>
+  <si>
+    <t>RH.1.HVT.W</t>
+  </si>
+  <si>
+    <t>TEST1</t>
+  </si>
+  <si>
+    <t>TEST2</t>
+  </si>
+  <si>
+    <t>TEST3</t>
+  </si>
+  <si>
+    <t>TEST4</t>
+  </si>
+  <si>
+    <t>CLIENT_SITE1</t>
+  </si>
+  <si>
+    <t>CLIENT_SITE2</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>192.168.1.2</t>
+  </si>
+  <si>
+    <t>192.168.1.3</t>
   </si>
 </sst>
 </file>
@@ -167,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,7 +198,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,19 +515,19 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="1" max="2" width="24.88671875" customWidth="1"/>
+    <col min="3" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -524,38 +544,44 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>5</v>
@@ -563,28 +589,60 @@
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -592,7 +650,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -600,7 +658,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -608,7 +666,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -616,7 +674,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -624,7 +682,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -632,7 +690,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -640,7 +698,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -648,7 +706,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -656,7 +714,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -664,7 +722,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -672,7 +730,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -680,7 +738,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -688,7 +746,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -696,7 +754,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -704,7 +762,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -712,7 +770,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -720,7 +778,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -728,7 +786,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -736,7 +794,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -744,7 +802,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -752,7 +810,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -760,7 +818,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -768,7 +826,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -776,7 +834,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -784,7 +842,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -792,7 +850,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -800,7 +858,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -808,7 +866,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -816,7 +874,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -824,7 +882,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -832,7 +890,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -840,7 +898,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -848,7 +906,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -856,7 +914,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -864,7 +922,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -872,7 +930,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -880,7 +938,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -888,7 +946,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -896,7 +954,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -904,7 +962,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -912,7 +970,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -920,7 +978,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -928,7 +986,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -936,7 +994,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -944,7 +1002,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -952,7 +1010,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -960,7 +1018,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -968,7 +1026,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -976,7 +1034,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -984,7 +1042,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -992,7 +1050,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1000,7 +1058,7 @@
       <c r="E57" s="3"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1008,7 +1066,7 @@
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1016,7 +1074,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1024,7 +1082,7 @@
       <c r="E60" s="3"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1032,7 +1090,7 @@
       <c r="E61" s="3"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1040,7 +1098,7 @@
       <c r="E62" s="3"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1048,7 +1106,7 @@
       <c r="E63" s="3"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1056,7 +1114,7 @@
       <c r="E64" s="3"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1064,7 +1122,7 @@
       <c r="E65" s="3"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1072,7 +1130,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1080,7 +1138,7 @@
       <c r="E67" s="3"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1088,7 +1146,7 @@
       <c r="E68" s="3"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -1096,7 +1154,7 @@
       <c r="E69" s="3"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -1104,7 +1162,7 @@
       <c r="E70" s="3"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1112,7 +1170,7 @@
       <c r="E71" s="3"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -1120,7 +1178,7 @@
       <c r="E72" s="3"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1128,7 +1186,7 @@
       <c r="E73" s="3"/>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1136,7 +1194,7 @@
       <c r="E74" s="3"/>
       <c r="F74" s="4"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1144,7 +1202,7 @@
       <c r="E75" s="3"/>
       <c r="F75" s="4"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1152,7 +1210,7 @@
       <c r="E76" s="3"/>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1160,7 +1218,7 @@
       <c r="E77" s="3"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1168,7 +1226,7 @@
       <c r="E78" s="3"/>
       <c r="F78" s="4"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -1176,7 +1234,7 @@
       <c r="E79" s="3"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -1184,7 +1242,7 @@
       <c r="E80" s="3"/>
       <c r="F80" s="4"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -1194,7 +1252,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E82:E1048576" xr:uid="{76097BCA-C432-4A7D-83F3-A52EE12AC1B8}">
       <formula1>"ios, nxos_ssh, eos"</formula1>
     </dataValidation>
@@ -1204,6 +1262,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E81" xr:uid="{4E2B1F9F-2EB5-4CD7-B5BA-8940E6AB7ED7}">
       <formula1>"cisco_ios, cisco_nxos, eos"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{6986AAFF-DDCA-465E-94AE-174B7731EDA8}">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>